<commit_message>
General Update JACK 4.SEPT.2072
9 Enemies completed and added.  Adjusted player position to starting location and added Note type script to the PlayerCapsule gameobject to let you know where to position the player for testing or actual game.  Added numerous more models.  Updated AI script.  Fixed numerous bugs.  Added Leaning.  Double tap lean to reset.  Enabled MainMenu under Canvas GameObject to let people see latest status of everything.
</commit_message>
<xml_diff>
--- a/Assets/npc_checklist.xlsx
+++ b/Assets/npc_checklist.xlsx
@@ -189,12 +189,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,7 +479,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,391 +517,401 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="3">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="2">
         <f>IFERROR(AVERAGE(C2:H2),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="4"/>
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="3">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="2">
         <f t="shared" ref="I3:I25" si="0">IFERROR(AVERAGE(C3:H3),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="3">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="4"/>
+      <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="3">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="4"/>
+      <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="3">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="4"/>
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="3">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="3">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2" t="s">
+      <c r="A10" s="4"/>
+      <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="3">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2" t="s">
+      <c r="A11" s="4"/>
+      <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="3">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2" t="s">
+      <c r="A12" s="4"/>
+      <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="3">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2" t="s">
+      <c r="A13" s="4"/>
+      <c r="B13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="3">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2" t="s">
+      <c r="A14" s="4"/>
+      <c r="B14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="3">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2" t="s">
+      <c r="A15" s="4"/>
+      <c r="B15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="3">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2" t="s">
+      <c r="A16" s="4"/>
+      <c r="B16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="3">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="3">
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2" t="s">
+      <c r="A18" s="4"/>
+      <c r="B18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="3">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2" t="s">
+      <c r="A19" s="4"/>
+      <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="3">
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2" t="s">
+      <c r="A20" s="4"/>
+      <c r="B20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="3">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="2" t="s">
+      <c r="A21" s="4"/>
+      <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="3">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2" t="s">
+      <c r="A22" s="4"/>
+      <c r="B22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="3">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2" t="s">
+      <c r="A23" s="4"/>
+      <c r="B23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="3">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2" t="s">
+      <c r="A24" s="4"/>
+      <c r="B24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="3">
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="2" t="s">
+      <c r="A25" s="4"/>
+      <c r="B25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="3">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>